<commit_message>
updates to api doc. refactor search and target wrappers
Signed-off-by: Solution Exchange <tdavis@opentext.com>
</commit_message>
<xml_diff>
--- a/api-doc/DSRestAPI.xlsx
+++ b/api-doc/DSRestAPI.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="17055" windowHeight="6345"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t>URL</t>
   </si>
@@ -93,13 +93,7 @@
     <t xml:space="preserve">root (no function or index) </t>
   </si>
   <si>
-    <t>url encoded VQL</t>
-  </si>
-  <si>
     <t>Query parmeters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group=*, locale=*, constraint=*, db-structure=* </t>
   </si>
   <si>
     <t>one or many parameters or attributes to construct a target DM (optional)</t>
@@ -183,25 +177,7 @@
     <t xml:space="preserve">TBD expose CoaContentFilter </t>
   </si>
   <si>
-    <t>Direct access to rdb connector (TBD)</t>
-  </si>
-  <si>
-    <t>Direct access to SOAP Webservice connector (TBD)</t>
-  </si>
-  <si>
-    <t>Direct access to Script Dynament (TBD)</t>
-  </si>
-  <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;</t>
-  </si>
-  <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/search?query=</t>
-  </si>
-  <si>
     <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/filter/</t>
-  </si>
-  <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/target?SEE QUERY Section</t>
   </si>
   <si>
     <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/content/</t>
@@ -219,13 +195,7 @@
     <t>Content Methods for a particular content item</t>
   </si>
   <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/contentgroup/&lt;%group_id%&gt;</t>
-  </si>
-  <si>
     <t>operations on one content group only</t>
-  </si>
-  <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/contentgroup/list</t>
   </si>
   <si>
     <t>list of content groups in this project</t>
@@ -270,66 +240,6 @@
     <t>Content</t>
   </si>
   <si>
-    <r>
-      <t>Functional Justification</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (see GET,POST,DELETE for functions) </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>POST</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (auth required)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">DELETE </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(auth required)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>QUERY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (syntax and guidelines)</t>
-    </r>
-  </si>
-  <si>
     <t>Security</t>
   </si>
   <si>
@@ -340,9 +250,6 @@
   </si>
   <si>
     <t>require auth for any write/delete</t>
-  </si>
-  <si>
-    <t>Connectors</t>
   </si>
   <si>
     <t>List content of a group</t>
@@ -360,32 +267,65 @@
     <t>liveserver/cps/rde/rest/&lt;%style%&gt;/http/</t>
   </si>
   <si>
-    <t>Direct access to HTTP Webservice connector (TBD)</t>
-  </si>
-  <si>
     <t>http://&lt;host&gt;:8080/cps/rde/xchg/base/hs.xsl/test/12345/?54321</t>
   </si>
   <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/cs/</t>
+    <t>query=*, engine=commonsearch|k2|ot7|api(*)</t>
   </si>
   <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/mm/</t>
+    <t xml:space="preserve">Functional Justification (see GET,POST,DELETE for functions) </t>
   </si>
   <si>
-    <t>Content Server</t>
+    <t>POST (auth required)</t>
   </si>
   <si>
-    <t>Media Management</t>
+    <t>DELETE (auth required)</t>
   </si>
   <si>
-    <t>query=*, engine=commonsearch|k2|ot7|api(*)</t>
+    <t>QUERY (syntax and guidelines)</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/contentgroup/list/</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/contentgroup/&lt;%group_id%&gt;/</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/search/</t>
+  </si>
+  <si>
+    <t>url encoded queries</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/target/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group=*, locale=*, constraint=*, db-structure=* , project=* </t>
+  </si>
+  <si>
+    <t>Direct access to rdb connector</t>
+  </si>
+  <si>
+    <t>Direct access to SOAP Webservice connector</t>
+  </si>
+  <si>
+    <t>Direct access to Script DynaMent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct access to HTTP Webservice connector </t>
+  </si>
+  <si>
+    <t>Connectors/Functions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,7 +364,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -471,6 +410,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -549,6 +493,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -583,6 +528,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -758,14 +704,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="102.5703125" customWidth="1"/>
     <col min="2" max="2" width="97.42578125" bestFit="1" customWidth="1"/>
@@ -776,254 +722,256 @@
     <col min="7" max="7" width="43.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1">
+    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F10" t="s">
-        <v>25</v>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>53</v>
       </c>
-      <c r="G10" t="s">
-        <v>104</v>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="3" t="s">
-        <v>60</v>
+    <row r="19" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>73</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="B21" t="s">
         <v>28</v>
       </c>
-      <c r="G13" t="s">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1">
-      <c r="A19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>32</v>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>43</v>
       </c>
-      <c r="D23" t="s">
-        <v>29</v>
-      </c>
+      <c r="B24" s="3"/>
     </row>
-    <row r="24" spans="1:4" s="1" customFormat="1">
-      <c r="A24" s="3" t="s">
+    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1">
-      <c r="A25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1">
-      <c r="A26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="1" customFormat="1">
+    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" s="1" customFormat="1">
-      <c r="A28" s="3" t="s">
-        <v>48</v>
+      <c r="F31" s="1" t="s">
+        <v>26</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>29</v>
+      <c r="G31" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="1" customFormat="1"/>
-    <row r="30" spans="1:4" s="1" customFormat="1">
-      <c r="A30" s="7" t="s">
-        <v>92</v>
+    <row r="32" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" s="1" customFormat="1">
-      <c r="A31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="1" customFormat="1">
-      <c r="A32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16384" s="1" customFormat="1">
+    <row r="33" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -17408,41 +17356,37 @@
       <c r="XFC33"/>
       <c r="XFD33"/>
     </row>
-    <row r="34" spans="1:16384" s="1" customFormat="1">
+    <row r="34" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>41</v>
       </c>
-      <c r="B34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16384" s="1" customFormat="1">
-      <c r="A35" t="s">
-        <v>42</v>
-      </c>
       <c r="B35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16384" s="1" customFormat="1">
-      <c r="A36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16384" s="1" customFormat="1">
-      <c r="A37" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:16384" s="1" customFormat="1"/>
-    <row r="39" spans="1:16384" s="1" customFormat="1"/>
-    <row r="40" spans="1:16384" s="1" customFormat="1"/>
+    <row r="36" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17450,30 +17394,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -17481,7 +17425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -17489,114 +17433,114 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="B11" t="s">
-        <v>53</v>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>73</v>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>77</v>
       </c>
-      <c r="B20" t="s">
-        <v>78</v>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -17606,24 +17550,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -17631,7 +17575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -17639,12 +17583,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
further updates to api to try to keep in sync with core development underway
Signed-off-by: Solution Exchange <tdavis@opentext.com>
</commit_message>
<xml_diff>
--- a/api-doc/DSRestAPI.xlsx
+++ b/api-doc/DSRestAPI.xlsx
@@ -102,9 +102,6 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>Content Methods</t>
-  </si>
-  <si>
     <t>List of contents (Target DM), and query parameters</t>
   </si>
   <si>
@@ -144,21 +141,6 @@
     <t>liveserver/cps/rde/rest/&lt;%style%&gt;/script/</t>
   </si>
   <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/content/&lt;%content_id%&gt;/attribute/&lt;%att_id%&gt;</t>
-  </si>
-  <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/content/&lt;%content_id%&gt;/constraints</t>
-  </si>
-  <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/content/&lt;%content_id%&gt;/comments</t>
-  </si>
-  <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/content/&lt;%content_id%&gt;/ratings</t>
-  </si>
-  <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/content/&lt;%content_id%&gt;/hits</t>
-  </si>
-  <si>
     <t>Mime-types:</t>
   </si>
   <si>
@@ -180,16 +162,10 @@
     <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/filter/</t>
   </si>
   <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/content/</t>
-  </si>
-  <si>
     <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/contentgroup/</t>
   </si>
   <si>
     <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/contentgroup/&lt;%group_id%&gt;/list</t>
-  </si>
-  <si>
-    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/project/&lt;%project_id%&gt;/content/&lt;%content_id%&gt;</t>
   </si>
   <si>
     <t>Content Methods for a particular content item</t>
@@ -319,6 +295,30 @@
   </si>
   <si>
     <t>Connectors/Functions</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/content/</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/content/&lt;%content_id%&gt;/attribute/&lt;%att_id%&gt;</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/content/&lt;%content_id%&gt;/constraints</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/content/&lt;%content_id%&gt;/comments</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/content/&lt;%content_id%&gt;/ratings</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/content/&lt;%content_id%&gt;/hits</t>
+  </si>
+  <si>
+    <t>liveserver/cps/rde/rest/&lt;%style%&gt;/content/?&lt;%content_id%&gt;</t>
+  </si>
+  <si>
+    <t>Content Methods all following items are query string now due to parsing conflicts with rewriting</t>
   </si>
 </sst>
 </file>
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,19 +727,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>25</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -763,12 +763,12 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -776,7 +776,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -784,12 +784,12 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
@@ -797,10 +797,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -813,13 +813,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -827,26 +827,26 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -855,27 +855,27 @@
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
@@ -883,22 +883,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>23</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>27</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>27</v>
@@ -926,41 +926,41 @@
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
         <v>15</v>
@@ -968,10 +968,10 @@
     </row>
     <row r="33" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -17358,26 +17358,26 @@
     </row>
     <row r="34" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:16384" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -17409,12 +17409,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -17435,10 +17435,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -17453,94 +17453,94 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>